<commit_message>
PA-28-181: Add 75% power curve for Pressure Altitude Vs. KCAS
</commit_message>
<xml_diff>
--- a/pa-28-181/pa-28-181.xlsx
+++ b/pa-28-181/pa-28-181.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbreslow/projects/open-aircraft-performance/pa-28-181/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251F4918-5224-7E49-844D-E505F357B584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4213285D-9AD2-E340-8C6B-51BA785B9035}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16580" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
+    <workbookView xWindow="20" yWindow="480" windowWidth="28800" windowHeight="16580" activeTab="2" xr2:uid="{2C93059D-7315-C048-801C-DCB81D215F85}"/>
   </bookViews>
   <sheets>
     <sheet name="KCAS Vs. % Power (Best Power)" sheetId="1" r:id="rId1"/>
     <sheet name="KCAS Vs. % Power (Best Eco)" sheetId="3" r:id="rId2"/>
-    <sheet name="Altitude Vs. KCAS at 65% (Eco)" sheetId="4" r:id="rId3"/>
+    <sheet name="Altitude Vs. KCAS" sheetId="4" r:id="rId3"/>
+    <sheet name="Altitude Vs. KCAS (No Fairings)" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Percent Power</t>
   </si>
@@ -43,16 +44,22 @@
     <t>Pressure Altitude</t>
   </si>
   <si>
-    <t>KTAS</t>
-  </si>
-  <si>
-    <t>KCAS</t>
-  </si>
-  <si>
     <t>KCAS (Peak EGT)</t>
   </si>
   <si>
     <t>KCAS (Best Power Mixture)</t>
+  </si>
+  <si>
+    <t>KTAS (65%)</t>
+  </si>
+  <si>
+    <t>KTAS (75%)</t>
+  </si>
+  <si>
+    <t>65% Power</t>
+  </si>
+  <si>
+    <t>75% Power</t>
   </si>
 </sst>
 </file>
@@ -96,9 +103,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,7 +1003,7 @@
                 <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
                 <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
               </a:rPr>
-              <a:t>Standard Day (ISA), Best Economy Mixture, 65% Power</a:t>
+              <a:t>Standard Day (ISA), Best Economy Mixture, Wheel Fairings Installed</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1026,15 +1034,142 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Altitude Vs. KCAS at 65% (Eco)'!$B$1</c:f>
+              <c:f>'Altitude Vs. KCAS'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>KCAS</c:v>
+                  <c:v>75% Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS'!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>114.998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114.32299999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114.119</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>114.24299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>113.739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.21299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112.551</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>112.663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112.066</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>111.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-59F9-3F4D-A579-74AA33461984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Altitude Vs. KCAS'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65% Power</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1060,43 +1195,9 @@
               </a:ln>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050">
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:backward val="0.2"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1200"/>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US"/>
-                      <a:t> </a:t>
-                    </a:r>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:trendline>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Altitude Vs. KCAS at 65% (Eco)'!$A$2:$A$14</c:f>
+              <c:f>'Altitude Vs. KCAS'!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1144,7 +1245,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Altitude Vs. KCAS at 65% (Eco)'!$B$2:$B$14</c:f>
+              <c:f>'Altitude Vs. KCAS'!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1336,6 +1437,23 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0">
+              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1355,7 +1473,543 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId2"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Pressure Altitude Vs. Calibrated Airspeed</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" b="0" i="0">
+                <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:rPr>
+              <a:t>Standard Day (ISA), Best Economy Mixture, Wheel Fairings Removed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.8306453225946247E-2"/>
+          <c:y val="0.19618456294903228"/>
+          <c:w val="0.91603312287064875"/>
+          <c:h val="0.77220754326797125"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Altitude Vs. KCAS (No Fairings)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>75% Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS (No Fairings)'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS (No Fairings)'!$C$2:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>106.998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>106.32299999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106.119</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>106.24299999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>105.739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>105.21299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>104.551</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>104.663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>104.066</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>103.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A3D-D945-A2FE-4975C9FF56C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Altitude Vs. KCAS (No Fairings)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>65% Power</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS (No Fairings)'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Altitude Vs. KCAS (No Fairings)'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>99.498000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.176000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.831000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.462000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>98.07</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>97.656000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97.218999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96.760999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>96.192999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>95.563000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94.83</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>94.084000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93.323999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5A3D-D945-A2FE-4975C9FF56C0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="951141263"/>
+        <c:axId val="948993503"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="951141263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="12000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="85000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="948993503"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2000"/>
+        <c:minorUnit val="1000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="948993503"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF">
+                <a:lumMod val="85000"/>
+              </a:sysClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="951141263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0">
+              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1715,84 +2369,46 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.08965</cdr:x>
-      <cdr:y>0.81532</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.37985</cdr:x>
-      <cdr:y>0.90966</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="6" name="TextBox 5">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>254002</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>461820</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>43076</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B289706-9784-ED4F-A8E0-BFD5877AA209}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CACBF4F0-503D-DE4C-9E85-75CCE1616C17}"/>
             </a:ext>
           </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="614820" y="3911478"/>
-          <a:ext cx="1990191" cy="452624"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" i="0">
-              <a:effectLst/>
-              <a:latin typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Gill Sans SemiBold" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-            </a:rPr>
-            <a:t>Note: </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0">
-              <a:effectLst/>
-              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-            </a:rPr>
-            <a:t>Subtract 8</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-            </a:rPr>
-            <a:t> KTS</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200" b="0" i="0">
-              <a:effectLst/>
-              <a:latin typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Gill Sans" panose="020B0502020104020203" pitchFamily="34" charset="-79"/>
-            </a:rPr>
-            <a:t> If Wheel Fairings Removed</a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2662,11 +3278,297 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride3.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4472C4"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="ED7D31"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="A5A5A5"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="FFC000"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="5B9BD5"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="70AD47"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0563C1"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="954F72"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック Light"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线 Light"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="游ゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="等线"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+      <a:font script="Armn" typeface="Arial"/>
+      <a:font script="Bugi" typeface="Leelawadee UI"/>
+      <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+      <a:font script="Java" typeface="Javanese Text"/>
+      <a:font script="Lisu" typeface="Segoe UI"/>
+      <a:font script="Mymr" typeface="Myanmar Text"/>
+      <a:font script="Nkoo" typeface="Ebrima"/>
+      <a:font script="Olck" typeface="Nirmala UI"/>
+      <a:font script="Osma" typeface="Ebrima"/>
+      <a:font script="Phag" typeface="Phagspa"/>
+      <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+      <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+      <a:font script="Syre" typeface="Estrangelo Edessa"/>
+      <a:font script="Sora" typeface="Nirmala UI"/>
+      <a:font script="Tale" typeface="Microsoft Tai Le"/>
+      <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+      <a:font script="Tfng" typeface="Ebrima"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="110000"/>
+              <a:satMod val="105000"/>
+              <a:tint val="67000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="103000"/>
+              <a:tint val="73000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="105000"/>
+              <a:satMod val="109000"/>
+              <a:tint val="81000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:satMod val="103000"/>
+              <a:lumMod val="102000"/>
+              <a:tint val="94000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:satMod val="110000"/>
+              <a:lumMod val="100000"/>
+              <a:shade val="100000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:lumMod val="99000"/>
+              <a:satMod val="120000"/>
+              <a:shade val="78000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst/>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147924CF-2EF1-8C42-B7BB-87C12FB00719}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -2682,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2732,7 +3634,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2747,7 +3649,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2788,8 +3690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8082DF-7D21-9148-B612-7759122ECC58}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2802,10 +3704,16 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2815,8 +3723,14 @@
       <c r="B2">
         <v>107.498</v>
       </c>
+      <c r="C2">
+        <v>114.998</v>
+      </c>
+      <c r="D2">
+        <v>107.5</v>
+      </c>
       <c r="E2">
-        <v>107.5</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2826,8 +3740,14 @@
       <c r="B3">
         <v>107.176</v>
       </c>
+      <c r="C3">
+        <v>114.32299999999999</v>
+      </c>
+      <c r="D3">
+        <v>108.75</v>
+      </c>
       <c r="E3">
-        <v>108.75</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2837,8 +3757,14 @@
       <c r="B4">
         <v>106.831</v>
       </c>
+      <c r="C4">
+        <v>114.119</v>
+      </c>
+      <c r="D4">
+        <v>110</v>
+      </c>
       <c r="E4">
-        <v>110</v>
+        <v>117.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2848,8 +3774,14 @@
       <c r="B5">
         <v>106.462</v>
       </c>
+      <c r="C5">
+        <v>114.24299999999999</v>
+      </c>
+      <c r="D5">
+        <v>111.25</v>
+      </c>
       <c r="E5">
-        <v>111.25</v>
+        <v>119.375</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2859,8 +3791,14 @@
       <c r="B6">
         <v>106.07</v>
       </c>
+      <c r="C6">
+        <v>113.739</v>
+      </c>
+      <c r="D6">
+        <v>112.5</v>
+      </c>
       <c r="E6">
-        <v>112.5</v>
+        <v>120.625</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2870,8 +3808,14 @@
       <c r="B7">
         <v>105.65600000000001</v>
       </c>
+      <c r="C7">
+        <v>113.21299999999999</v>
+      </c>
+      <c r="D7">
+        <v>113.75</v>
+      </c>
       <c r="E7">
-        <v>113.75</v>
+        <v>121.875</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -2881,8 +3825,14 @@
       <c r="B8">
         <v>105.21899999999999</v>
       </c>
+      <c r="C8">
+        <v>112.551</v>
+      </c>
+      <c r="D8">
+        <v>115</v>
+      </c>
       <c r="E8">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2892,8 +3842,14 @@
       <c r="B9">
         <v>104.761</v>
       </c>
+      <c r="C9">
+        <v>112.663</v>
+      </c>
+      <c r="D9">
+        <v>116.25</v>
+      </c>
       <c r="E9">
-        <v>116.25</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -2903,8 +3859,14 @@
       <c r="B10">
         <v>104.193</v>
       </c>
+      <c r="C10">
+        <v>112.066</v>
+      </c>
+      <c r="D10">
+        <v>117.4</v>
+      </c>
       <c r="E10">
-        <v>117.4</v>
+        <v>126.25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -2914,8 +3876,14 @@
       <c r="B11">
         <v>103.563</v>
       </c>
+      <c r="C11">
+        <v>111.45</v>
+      </c>
+      <c r="D11">
+        <v>118.5</v>
+      </c>
       <c r="E11">
-        <v>118.5</v>
+        <v>127.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2925,7 +3893,7 @@
       <c r="B12">
         <v>102.83</v>
       </c>
-      <c r="E12">
+      <c r="D12">
         <v>119.5</v>
       </c>
     </row>
@@ -2936,7 +3904,7 @@
       <c r="B13">
         <v>102.084</v>
       </c>
-      <c r="E13">
+      <c r="D13">
         <v>120.5</v>
       </c>
     </row>
@@ -2947,8 +3915,174 @@
       <c r="B14">
         <v>101.324</v>
       </c>
-      <c r="E14">
+      <c r="D14">
         <v>121.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F54C2C-149E-4647-BD57-1BCE1199BF0F}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>99.498000000000005</v>
+      </c>
+      <c r="C2">
+        <v>106.998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3">
+        <v>99.176000000000002</v>
+      </c>
+      <c r="C3">
+        <v>106.32299999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>98.831000000000003</v>
+      </c>
+      <c r="C4">
+        <v>106.119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3000</v>
+      </c>
+      <c r="B5">
+        <v>98.462000000000003</v>
+      </c>
+      <c r="C5">
+        <v>106.24299999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4000</v>
+      </c>
+      <c r="B6">
+        <v>98.07</v>
+      </c>
+      <c r="C6">
+        <v>105.739</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+      <c r="B7">
+        <v>97.656000000000006</v>
+      </c>
+      <c r="C7">
+        <v>105.21299999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6000</v>
+      </c>
+      <c r="B8">
+        <v>97.218999999999994</v>
+      </c>
+      <c r="C8">
+        <v>104.551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7000</v>
+      </c>
+      <c r="B9">
+        <v>96.760999999999996</v>
+      </c>
+      <c r="C9">
+        <v>104.663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8000</v>
+      </c>
+      <c r="B10">
+        <v>96.192999999999998</v>
+      </c>
+      <c r="C10">
+        <v>104.066</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9000</v>
+      </c>
+      <c r="B11">
+        <v>95.563000000000002</v>
+      </c>
+      <c r="C11">
+        <v>103.45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10000</v>
+      </c>
+      <c r="B12">
+        <v>94.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11000</v>
+      </c>
+      <c r="B13">
+        <v>94.084000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12000</v>
+      </c>
+      <c r="B14">
+        <v>93.323999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>